<commit_message>
change category to 'Presentation'
</commit_message>
<xml_diff>
--- a/data/pre2018_summary.xlsx
+++ b/data/pre2018_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/haerther_metrics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816A39D0-31C9-9E41-B8D1-7C95EB60B879}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CDF528-446B-1440-A06E-6CD154D08B36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="2420" windowWidth="26040" windowHeight="14540" xr2:uid="{C0DC303A-DE82-5B40-A7FA-30B71FF9166A}"/>
   </bookViews>
@@ -72,7 +72,7 @@
     <t>Media opportunity</t>
   </si>
   <si>
-    <t>Conference or active meeting</t>
+    <t>Presentation</t>
   </si>
 </sst>
 </file>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA96190-A5FA-7640-BFF8-ABC43EC5AF22}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>